<commit_message>
transport limit h2 pipeline implemented
</commit_message>
<xml_diff>
--- a/pipeline_limits.xlsx
+++ b/pipeline_limits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Code_Projekte\GitHub\hydro_opt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Code\hydro_opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CFD430-7ABF-4A3B-AAAE-62E77EAE4158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4304D91-2FCD-49D4-B003-C3705464B5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2045_level_2" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="245">
   <si>
     <t>To Country</t>
   </si>
@@ -775,6 +775,9 @@
   </si>
   <si>
     <t>To Code</t>
+  </si>
+  <si>
+    <t>MWh/y</t>
   </si>
 </sst>
 </file>
@@ -1237,15 +1240,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A31CF60-1646-4F5D-B575-B081E039D32D}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="Q80" sqref="Q80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1261,8 +1264,11 @@
       <c r="E1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1278,8 +1284,12 @@
       <c r="E2">
         <v>448</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>E2*1000*365</f>
+        <v>163520000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1295,8 +1305,12 @@
       <c r="E3">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">E3*1000*365</f>
+        <v>89425000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1312,8 +1326,12 @@
       <c r="E4">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>54750000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1329,8 +1347,12 @@
       <c r="E5">
         <v>219</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>79935000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1346,8 +1368,12 @@
       <c r="E6">
         <v>156</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>56940000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1363,8 +1389,12 @@
       <c r="E7">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>12045000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1380,8 +1410,12 @@
       <c r="E8">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1397,8 +1431,12 @@
       <c r="E9">
         <v>105.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>38507500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1414,8 +1452,12 @@
       <c r="E10">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>6205000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1431,8 +1473,12 @@
       <c r="E11">
         <v>216</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>78840000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1448,8 +1494,12 @@
       <c r="E12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1465,8 +1515,12 @@
       <c r="E13">
         <v>43.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>15877500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1482,8 +1536,12 @@
       <c r="E14">
         <v>83.983499999999992</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>30653977.499999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1499,8 +1557,12 @@
       <c r="E15">
         <v>125.08641950000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>45656543.1175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1516,8 +1578,12 @@
       <c r="E16">
         <v>43.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>15877500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1533,8 +1599,12 @@
       <c r="E17">
         <v>128.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>46866000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1550,8 +1620,12 @@
       <c r="E18">
         <v>63.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>23287000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1567,8 +1641,12 @@
       <c r="E19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>5840000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1584,8 +1662,12 @@
       <c r="E20">
         <v>231.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>84534000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1601,8 +1683,12 @@
       <c r="E21">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>10950000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1618,8 +1704,12 @@
       <c r="E22">
         <v>156</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>56940000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1635,8 +1725,12 @@
       <c r="E23">
         <v>290</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>105850000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1652,8 +1746,12 @@
       <c r="E24">
         <v>200</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1669,8 +1767,12 @@
       <c r="E25">
         <v>200</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1686,8 +1788,12 @@
       <c r="E26">
         <v>200</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1703,8 +1809,12 @@
       <c r="E27">
         <v>504</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>183960000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1720,8 +1830,12 @@
       <c r="E28">
         <v>910</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>332150000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1737,8 +1851,12 @@
       <c r="E29">
         <v>200</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1754,8 +1872,12 @@
       <c r="E30">
         <v>243</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>88695000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1771,8 +1893,12 @@
       <c r="E31">
         <v>216</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>78840000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1788,8 +1914,12 @@
       <c r="E32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>36500000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1805,8 +1935,12 @@
       <c r="E33">
         <v>150</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>54750000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1822,8 +1956,12 @@
       <c r="E34">
         <v>105.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>38507500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1839,8 +1977,12 @@
       <c r="E35">
         <v>231.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>84534000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1856,8 +1998,12 @@
       <c r="E36">
         <v>290</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>105850000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1873,8 +2019,12 @@
       <c r="E37">
         <v>504</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>183960000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1890,8 +2040,12 @@
       <c r="E38">
         <v>243</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>88695000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1907,8 +2061,12 @@
       <c r="E39">
         <v>469.6</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>171404000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1924,8 +2082,12 @@
       <c r="E40">
         <v>173.57168999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>63353666.850000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1941,8 +2103,12 @@
       <c r="E41">
         <v>204</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>74460000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1958,8 +2124,12 @@
       <c r="E42">
         <v>81.753999999999991</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>29840209.999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1975,8 +2145,12 @@
       <c r="E43">
         <v>128.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>46866000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -1992,8 +2166,12 @@
       <c r="E44">
         <v>153.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>56064000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2009,8 +2187,12 @@
       <c r="E45">
         <v>200</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -2026,8 +2208,12 @@
       <c r="E46">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>7154000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2043,8 +2229,12 @@
       <c r="E47">
         <v>18.244730499999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>6659326.6324999994</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2060,8 +2250,12 @@
       <c r="E48">
         <v>168</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>61320000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2077,8 +2271,12 @@
       <c r="E49">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>7154000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2094,8 +2292,12 @@
       <c r="E50">
         <v>88</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>32120000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -2111,8 +2313,12 @@
       <c r="E51">
         <v>113.3796505</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>41383572.432500005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -2128,8 +2334,12 @@
       <c r="E52">
         <v>200</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -2145,8 +2355,12 @@
       <c r="E53">
         <v>186.9496915</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>68236637.397499993</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -2162,8 +2376,12 @@
       <c r="E54">
         <v>200</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2179,8 +2397,12 @@
       <c r="E55">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>6205000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -2196,8 +2418,12 @@
       <c r="E56">
         <v>216</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>78840000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2213,8 +2439,12 @@
       <c r="E57">
         <v>469.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>171367500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -2230,8 +2460,12 @@
       <c r="E58">
         <v>200</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2247,8 +2481,12 @@
       <c r="E59">
         <v>414</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>151110000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2264,8 +2502,12 @@
       <c r="E60">
         <v>30</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>10950000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -2281,8 +2523,12 @@
       <c r="E61">
         <v>213.57168999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>77953666.849999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -2298,8 +2544,12 @@
       <c r="E62">
         <v>171.50922800000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>62600868.219999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -2315,8 +2565,12 @@
       <c r="E63">
         <v>81</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>29565000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>21</v>
       </c>
@@ -2332,8 +2586,12 @@
       <c r="E64">
         <v>125.08641950000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>45656543.1175</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>21</v>
       </c>
@@ -2349,8 +2607,12 @@
       <c r="E65">
         <v>153.6</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>56064000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -2366,8 +2628,12 @@
       <c r="E66">
         <v>63.8</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>23287000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -2383,8 +2649,12 @@
       <c r="E67">
         <v>156</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <f t="shared" ref="F67:F85" si="1">E67*1000*365</f>
+        <v>56940000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2400,8 +2670,12 @@
       <c r="E68">
         <v>156</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>56940000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -2417,8 +2691,12 @@
       <c r="E69">
         <v>200</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -2434,8 +2712,12 @@
       <c r="E70">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>5840000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -2451,8 +2733,12 @@
       <c r="E71">
         <v>33</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>12045000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -2468,8 +2754,12 @@
       <c r="E72">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>7154000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -2485,8 +2775,12 @@
       <c r="E73">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>7154000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -2502,8 +2796,12 @@
       <c r="E74">
         <v>216</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>78840000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -2519,8 +2817,12 @@
       <c r="E75">
         <v>320</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>116800000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -2536,8 +2838,12 @@
       <c r="E76">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>29565000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -2553,8 +2859,12 @@
       <c r="E77">
         <v>910</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>332150000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>36</v>
       </c>
@@ -2570,8 +2880,12 @@
       <c r="E78">
         <v>150</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>54750000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -2587,8 +2901,12 @@
       <c r="E79">
         <v>171.8</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>62707000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -2604,8 +2922,12 @@
       <c r="E80">
         <v>312</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>113880000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -2621,8 +2943,12 @@
       <c r="E81">
         <v>200</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -2638,8 +2964,12 @@
       <c r="E82">
         <v>18.244730499999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>6659326.6324999994</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2655,8 +2985,12 @@
       <c r="E83">
         <v>100</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>36500000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -2672,8 +3006,12 @@
       <c r="E84">
         <v>204</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>74460000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -2688,6 +3026,10 @@
       </c>
       <c r="E85">
         <v>135</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>49275000</v>
       </c>
     </row>
   </sheetData>
@@ -2700,13 +3042,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T169"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection sqref="A1:N169"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -2741,6 +3083,9 @@
       <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
       <c r="S1" t="s">
         <v>3</v>
       </c>
@@ -2748,7 +3093,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -2793,7 +3138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -2838,7 +3183,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -2883,7 +3228,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2928,7 +3273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -2973,7 +3318,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -3018,7 +3363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -3063,7 +3408,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -3108,7 +3453,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -3153,7 +3498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -3198,7 +3543,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -3243,7 +3588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -3288,7 +3633,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
@@ -3333,7 +3678,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3723,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -3423,7 +3768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -3468,7 +3813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -3513,7 +3858,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -3558,7 +3903,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -3603,7 +3948,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -3648,7 +3993,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -3693,7 +4038,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>12</v>
       </c>
@@ -3738,7 +4083,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>17</v>
       </c>
@@ -3783,7 +4128,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>17</v>
       </c>
@@ -3828,7 +4173,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3873,7 +4218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>19</v>
       </c>
@@ -3918,7 +4263,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
@@ -3963,7 +4308,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>19</v>
       </c>
@@ -4008,7 +4353,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -4053,7 +4398,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -4098,7 +4443,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -4143,7 +4488,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -4188,7 +4533,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -4233,7 +4578,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -4278,7 +4623,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -4323,7 +4668,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>18</v>
       </c>
@@ -4368,7 +4713,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>24</v>
       </c>
@@ -4413,7 +4758,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>24</v>
       </c>
@@ -4458,7 +4803,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
@@ -4503,7 +4848,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -4548,7 +4893,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>24</v>
       </c>
@@ -4593,7 +4938,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>24</v>
       </c>
@@ -4638,7 +4983,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>26</v>
       </c>
@@ -4683,7 +5028,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>26</v>
       </c>
@@ -4728,7 +5073,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>27</v>
       </c>
@@ -4773,7 +5118,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>27</v>
       </c>
@@ -4818,7 +5163,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>27</v>
       </c>
@@ -4863,7 +5208,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>27</v>
       </c>
@@ -4908,7 +5253,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>28</v>
       </c>
@@ -4953,7 +5298,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>28</v>
       </c>
@@ -4998,7 +5343,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>28</v>
       </c>
@@ -5043,7 +5388,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>28</v>
       </c>
@@ -5088,7 +5433,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -5133,7 +5478,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>28</v>
       </c>
@@ -5178,7 +5523,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>13</v>
       </c>
@@ -5223,7 +5568,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>13</v>
       </c>
@@ -5268,7 +5613,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>13</v>
       </c>
@@ -5313,7 +5658,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>13</v>
       </c>
@@ -5358,7 +5703,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>13</v>
       </c>
@@ -5403,7 +5748,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5793,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>13</v>
       </c>
@@ -5493,7 +5838,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>13</v>
       </c>
@@ -5538,7 +5883,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>9</v>
       </c>
@@ -5583,7 +5928,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>9</v>
       </c>
@@ -5628,7 +5973,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>9</v>
       </c>
@@ -5673,7 +6018,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
@@ -5718,7 +6063,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
@@ -5763,7 +6108,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>9</v>
       </c>
@@ -5808,7 +6153,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
@@ -5853,7 +6198,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>9</v>
       </c>
@@ -5898,7 +6243,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
@@ -5943,7 +6288,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
@@ -5988,7 +6333,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>9</v>
       </c>
@@ -6033,7 +6378,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>9</v>
       </c>
@@ -6078,7 +6423,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>9</v>
       </c>
@@ -6123,7 +6468,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>9</v>
       </c>
@@ -6168,7 +6513,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>9</v>
       </c>
@@ -6213,7 +6558,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>9</v>
       </c>
@@ -6258,7 +6603,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
@@ -6303,7 +6648,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>9</v>
       </c>
@@ -6348,7 +6693,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>20</v>
       </c>
@@ -6393,7 +6738,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>20</v>
       </c>
@@ -6438,7 +6783,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>22</v>
       </c>
@@ -6483,7 +6828,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>22</v>
       </c>
@@ -6528,7 +6873,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>22</v>
       </c>
@@ -6573,7 +6918,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>22</v>
       </c>
@@ -6618,7 +6963,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>22</v>
       </c>
@@ -6663,7 +7008,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>22</v>
       </c>
@@ -6708,7 +7053,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>22</v>
       </c>
@@ -6753,7 +7098,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>22</v>
       </c>
@@ -6798,7 +7143,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>32</v>
       </c>
@@ -6843,7 +7188,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>40</v>
       </c>
@@ -6888,7 +7233,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>4</v>
       </c>
@@ -6933,7 +7278,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>4</v>
       </c>
@@ -6978,7 +7323,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>4</v>
       </c>
@@ -7023,7 +7368,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
@@ -7068,7 +7413,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>4</v>
       </c>
@@ -7113,7 +7458,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>4</v>
       </c>
@@ -7158,7 +7503,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>29</v>
       </c>
@@ -7203,7 +7548,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>29</v>
       </c>
@@ -7248,7 +7593,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>29</v>
       </c>
@@ -7293,7 +7638,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>29</v>
       </c>
@@ -7338,7 +7683,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>33</v>
       </c>
@@ -7383,7 +7728,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>33</v>
       </c>
@@ -7428,7 +7773,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>33</v>
       </c>
@@ -7473,7 +7818,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>33</v>
       </c>
@@ -7518,7 +7863,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>14</v>
       </c>
@@ -7563,7 +7908,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>14</v>
       </c>
@@ -7608,7 +7953,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>15</v>
       </c>
@@ -7653,7 +7998,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>15</v>
       </c>
@@ -7698,7 +8043,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>15</v>
       </c>
@@ -7743,7 +8088,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>15</v>
       </c>
@@ -7788,7 +8133,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>34</v>
       </c>
@@ -7827,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>34</v>
       </c>
@@ -7866,7 +8211,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>34</v>
       </c>
@@ -7905,7 +8250,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>34</v>
       </c>
@@ -7944,7 +8289,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
         <v>25</v>
       </c>
@@ -7983,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>25</v>
       </c>
@@ -8022,7 +8367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>25</v>
       </c>
@@ -8061,7 +8406,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>25</v>
       </c>
@@ -8100,7 +8445,7 @@
         <v>213.57168999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>25</v>
       </c>
@@ -8139,7 +8484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>25</v>
       </c>
@@ -8178,7 +8523,7 @@
         <v>171.50922800000001</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>35</v>
       </c>
@@ -8217,7 +8562,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>35</v>
       </c>
@@ -8256,7 +8601,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>21</v>
       </c>
@@ -8295,7 +8640,7 @@
         <v>110.73</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>21</v>
       </c>
@@ -8334,7 +8679,7 @@
         <v>125.08641950000001</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>21</v>
       </c>
@@ -8373,7 +8718,7 @@
         <v>153.6</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>21</v>
       </c>
@@ -8412,7 +8757,7 @@
         <v>153.6</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
         <v>23</v>
       </c>
@@ -8451,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>23</v>
       </c>
@@ -8490,7 +8835,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>10</v>
       </c>
@@ -8529,7 +8874,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>10</v>
       </c>
@@ -8568,7 +8913,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>10</v>
       </c>
@@ -8607,7 +8952,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>10</v>
       </c>
@@ -8646,7 +8991,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>10</v>
       </c>
@@ -8685,7 +9030,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>10</v>
       </c>
@@ -8724,7 +9069,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>11</v>
       </c>
@@ -8763,7 +9108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>11</v>
       </c>
@@ -8802,7 +9147,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>11</v>
       </c>
@@ -8841,7 +9186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>11</v>
       </c>
@@ -8880,7 +9225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>11</v>
       </c>
@@ -8919,7 +9264,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>11</v>
       </c>
@@ -8958,7 +9303,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>11</v>
       </c>
@@ -8997,7 +9342,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>11</v>
       </c>
@@ -9036,7 +9381,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>7</v>
       </c>
@@ -9075,7 +9420,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>7</v>
       </c>
@@ -9114,7 +9459,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>7</v>
       </c>
@@ -9153,7 +9498,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>7</v>
       </c>
@@ -9192,7 +9537,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>7</v>
       </c>
@@ -9231,7 +9576,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>7</v>
       </c>
@@ -9270,7 +9615,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>30</v>
       </c>
@@ -9309,7 +9654,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>30</v>
       </c>
@@ -9348,7 +9693,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>36</v>
       </c>
@@ -9387,7 +9732,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>36</v>
       </c>
@@ -9426,7 +9771,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>36</v>
       </c>
@@ -9465,7 +9810,7 @@
         <v>171.8</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>36</v>
       </c>
@@ -9504,7 +9849,7 @@
         <v>171.8</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>36</v>
       </c>
@@ -9543,7 +9888,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>36</v>
       </c>
@@ -9582,7 +9927,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>16</v>
       </c>
@@ -9621,7 +9966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>39</v>
       </c>
@@ -9660,7 +10005,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>16</v>
       </c>
@@ -9699,7 +10044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>39</v>
       </c>
@@ -9738,7 +10083,7 @@
         <v>18.244730499999999</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
         <v>31</v>
       </c>
@@ -9777,7 +10122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>31</v>
       </c>
@@ -9816,7 +10161,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>31</v>
       </c>
@@ -9855,7 +10200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>31</v>
       </c>
@@ -9894,7 +10239,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>31</v>
       </c>
@@ -9933,7 +10278,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>31</v>
       </c>
@@ -9982,126 +10327,41 @@
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <mergeCells count="169">
-    <mergeCell ref="E169:G169"/>
-    <mergeCell ref="E163:G163"/>
-    <mergeCell ref="E164:G164"/>
-    <mergeCell ref="E165:G165"/>
-    <mergeCell ref="E166:G166"/>
-    <mergeCell ref="E167:G167"/>
-    <mergeCell ref="E168:G168"/>
-    <mergeCell ref="E157:G157"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="E159:G159"/>
-    <mergeCell ref="E160:G160"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="E162:G162"/>
-    <mergeCell ref="E152:G152"/>
-    <mergeCell ref="E153:G153"/>
-    <mergeCell ref="E154:G154"/>
-    <mergeCell ref="E155:G155"/>
-    <mergeCell ref="E156:G156"/>
-    <mergeCell ref="E146:G146"/>
-    <mergeCell ref="E147:G147"/>
-    <mergeCell ref="E148:G148"/>
-    <mergeCell ref="E149:G149"/>
-    <mergeCell ref="E150:G150"/>
-    <mergeCell ref="E151:G151"/>
-    <mergeCell ref="E140:G140"/>
-    <mergeCell ref="E141:G141"/>
-    <mergeCell ref="E142:G142"/>
-    <mergeCell ref="E143:G143"/>
-    <mergeCell ref="E144:G144"/>
-    <mergeCell ref="E145:G145"/>
-    <mergeCell ref="E134:G134"/>
-    <mergeCell ref="E135:G135"/>
-    <mergeCell ref="E136:G136"/>
-    <mergeCell ref="E137:G137"/>
-    <mergeCell ref="E138:G138"/>
-    <mergeCell ref="E139:G139"/>
-    <mergeCell ref="E129:G129"/>
-    <mergeCell ref="E130:G130"/>
-    <mergeCell ref="E131:G131"/>
-    <mergeCell ref="E132:G132"/>
-    <mergeCell ref="E133:G133"/>
-    <mergeCell ref="E124:G124"/>
-    <mergeCell ref="E125:G125"/>
-    <mergeCell ref="E126:G126"/>
-    <mergeCell ref="E127:G127"/>
-    <mergeCell ref="E128:G128"/>
-    <mergeCell ref="E118:G118"/>
-    <mergeCell ref="E119:G119"/>
-    <mergeCell ref="E120:G120"/>
-    <mergeCell ref="E121:G121"/>
-    <mergeCell ref="E122:G122"/>
-    <mergeCell ref="E123:G123"/>
-    <mergeCell ref="E113:G113"/>
-    <mergeCell ref="E114:G114"/>
-    <mergeCell ref="E115:G115"/>
-    <mergeCell ref="E116:G116"/>
-    <mergeCell ref="E117:G117"/>
-    <mergeCell ref="E108:G108"/>
-    <mergeCell ref="E109:G109"/>
-    <mergeCell ref="E110:G110"/>
-    <mergeCell ref="E111:G111"/>
-    <mergeCell ref="E112:G112"/>
-    <mergeCell ref="E104:G104"/>
-    <mergeCell ref="E105:G105"/>
-    <mergeCell ref="E106:G106"/>
-    <mergeCell ref="E107:G107"/>
-    <mergeCell ref="E100:G100"/>
-    <mergeCell ref="E101:G101"/>
-    <mergeCell ref="E102:G102"/>
-    <mergeCell ref="E103:G103"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
     <mergeCell ref="E46:G46"/>
     <mergeCell ref="E47:G47"/>
     <mergeCell ref="E48:G48"/>
@@ -10116,41 +10376,126 @@
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="E40:G40"/>
     <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="E100:G100"/>
+    <mergeCell ref="E101:G101"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="E103:G103"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="E108:G108"/>
+    <mergeCell ref="E109:G109"/>
+    <mergeCell ref="E110:G110"/>
+    <mergeCell ref="E111:G111"/>
+    <mergeCell ref="E112:G112"/>
+    <mergeCell ref="E104:G104"/>
+    <mergeCell ref="E105:G105"/>
+    <mergeCell ref="E106:G106"/>
+    <mergeCell ref="E107:G107"/>
+    <mergeCell ref="E118:G118"/>
+    <mergeCell ref="E119:G119"/>
+    <mergeCell ref="E120:G120"/>
+    <mergeCell ref="E121:G121"/>
+    <mergeCell ref="E122:G122"/>
+    <mergeCell ref="E123:G123"/>
+    <mergeCell ref="E113:G113"/>
+    <mergeCell ref="E114:G114"/>
+    <mergeCell ref="E115:G115"/>
+    <mergeCell ref="E116:G116"/>
+    <mergeCell ref="E117:G117"/>
+    <mergeCell ref="E129:G129"/>
+    <mergeCell ref="E130:G130"/>
+    <mergeCell ref="E131:G131"/>
+    <mergeCell ref="E132:G132"/>
+    <mergeCell ref="E133:G133"/>
+    <mergeCell ref="E124:G124"/>
+    <mergeCell ref="E125:G125"/>
+    <mergeCell ref="E126:G126"/>
+    <mergeCell ref="E127:G127"/>
+    <mergeCell ref="E128:G128"/>
+    <mergeCell ref="E140:G140"/>
+    <mergeCell ref="E141:G141"/>
+    <mergeCell ref="E142:G142"/>
+    <mergeCell ref="E143:G143"/>
+    <mergeCell ref="E144:G144"/>
+    <mergeCell ref="E145:G145"/>
+    <mergeCell ref="E134:G134"/>
+    <mergeCell ref="E135:G135"/>
+    <mergeCell ref="E136:G136"/>
+    <mergeCell ref="E137:G137"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="E139:G139"/>
+    <mergeCell ref="E152:G152"/>
+    <mergeCell ref="E153:G153"/>
+    <mergeCell ref="E154:G154"/>
+    <mergeCell ref="E155:G155"/>
+    <mergeCell ref="E156:G156"/>
+    <mergeCell ref="E146:G146"/>
+    <mergeCell ref="E147:G147"/>
+    <mergeCell ref="E148:G148"/>
+    <mergeCell ref="E149:G149"/>
+    <mergeCell ref="E150:G150"/>
+    <mergeCell ref="E151:G151"/>
+    <mergeCell ref="E169:G169"/>
+    <mergeCell ref="E163:G163"/>
+    <mergeCell ref="E164:G164"/>
+    <mergeCell ref="E165:G165"/>
+    <mergeCell ref="E166:G166"/>
+    <mergeCell ref="E167:G167"/>
+    <mergeCell ref="E168:G168"/>
+    <mergeCell ref="E157:G157"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="E159:G159"/>
+    <mergeCell ref="E160:G160"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="E162:G162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>